<commit_message>
WAY Corrector - تحديث الملف: 24/11/2025, 15:31:00
</commit_message>
<xml_diff>
--- a/MCQ8.xlsx
+++ b/MCQ8.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -437,10 +437,45 @@
         <v>اسم التصنيف</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>سؤال</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+      <c r="D2" t="str">
+        <v>3</v>
+      </c>
+      <c r="E2" t="str">
+        <v>4</v>
+      </c>
+      <c r="F2" t="str">
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
+        <v>5</v>
+      </c>
+      <c r="H2" t="str">
+        <v>واو</v>
+      </c>
+      <c r="I2" t="str">
+        <v>علوم</v>
+      </c>
+      <c r="J2" t="str">
+        <v>الاول</v>
+      </c>
+      <c r="K2" t="str">
+        <v>جلد</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>